<commit_message>
- JMeter / Visual VM Messung hinzugefügt
</commit_message>
<xml_diff>
--- a/docs/JMeter_Requests_Size.xlsx
+++ b/docs/JMeter_Requests_Size.xlsx
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>